<commit_message>
Manual VIES search included in error handling for API, readme added
</commit_message>
<xml_diff>
--- a/testdata1.xlsx
+++ b/testdata1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piers\automation\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piers\automation\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66419D8-2631-402D-B429-1A798CE6DDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63E4A9-BD3C-452F-A415-B9B3C9B2A2D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="2475" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>VAT Number</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Randstad Holding Limited</t>
+  </si>
+  <si>
+    <t>RANDSTAD PUBLIC SERVICES LIMITED</t>
+  </si>
+  <si>
+    <t>MANPOWER UK HOLDINGS LIMITED</t>
   </si>
 </sst>
 </file>
@@ -408,113 +414,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>154186115</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>154186115</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>154186115</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>